<commit_message>
set it so email goes to right place
</commit_message>
<xml_diff>
--- a/AssessAutomation/customer.xlsx
+++ b/AssessAutomation/customer.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Rev\week7\assessment\AssessAutomation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\ConnerKnight_Automation_Challenge1\AssessAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920797C5-A600-46D0-BDA5-2FA123547F90}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEE8F41-4EA0-425B-A29A-EB8B45B2CFFE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5628" xr2:uid="{9D51EA8A-1DE4-4731-A055-ECFCF6027D27}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5628" xr2:uid="{9D51EA8A-1DE4-4731-A055-ECFCF6027D27}"/>
   </bookViews>
   <sheets>
     <sheet name="userinfo" sheetId="2" r:id="rId1"/>
@@ -26,69 +26,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
-  <si>
-    <t>Chris</t>
-  </si>
-  <si>
-    <t>Jones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChrisSJones@dayrep.com </t>
-  </si>
-  <si>
-    <t>530-631-8725</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1290 Eagles Nest Drive. Sacramento, CA 95814 </t>
-  </si>
-  <si>
-    <t>Mikrotechnic</t>
-  </si>
-  <si>
-    <t>Manpower development specialist</t>
-  </si>
-  <si>
-    <t>George</t>
-  </si>
-  <si>
-    <t>Cordeiro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GeorgeBCordeiro@dayrep.com </t>
-  </si>
-  <si>
-    <t>267-294-3132</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2618 Valley Drive. Philadelphia, PA 19108 </t>
-  </si>
-  <si>
-    <t>Endicott Johnson</t>
-  </si>
-  <si>
-    <t>Floral designer</t>
-  </si>
-  <si>
-    <t>Roy</t>
-  </si>
-  <si>
-    <t>Fuller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RoyEFuller@rhyta.com </t>
-  </si>
-  <si>
-    <t>304-885-0638</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2049 Kelly Drive. Frederick, WV 21701 </t>
-  </si>
-  <si>
-    <t>Auto Palace</t>
-  </si>
-  <si>
-    <t>Real estate appraiser</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Role in Company</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Roger</t>
+  </si>
+  <si>
+    <t>Huffman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RogerLHuffman@armyspy.com </t>
+  </si>
+  <si>
+    <t>619-675-5903</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2299 Grim Avenue. San Diego, CA 92103 </t>
+  </si>
+  <si>
+    <t>Heilig-Meyers</t>
+  </si>
+  <si>
+    <t>Floor finisher</t>
+  </si>
+  <si>
+    <t>Vesta</t>
+  </si>
+  <si>
+    <t>McAteer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VestaEMcAteer@jourrapide.com </t>
+  </si>
+  <si>
+    <t>253-520-6265</t>
+  </si>
+  <si>
+    <t xml:space="preserve">115 Horizon Circle. Kent, WA 98031 </t>
+  </si>
+  <si>
+    <t>Disc Jockey</t>
+  </si>
+  <si>
+    <t>Telecommunications specialist</t>
+  </si>
+  <si>
+    <t>Laurie</t>
+  </si>
+  <si>
+    <t>Strand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LaurieLStrand@rhyta.com </t>
+  </si>
+  <si>
+    <t>901-870-5509</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3130 Gladwell Street. Memphis, TN 38133 </t>
+  </si>
+  <si>
+    <t>Total Yard Management</t>
+  </si>
+  <si>
+    <t>Loss prevention agent</t>
   </si>
   <si>
     <t>success</t>
@@ -484,82 +508,85 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>